<commit_message>
added the master excel file
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/Visium_IF_SCZ_PNN_1stRound_08142022_MasterExcel.xlsx
+++ b/raw-data/sample_info/Visium_IF_SCZ_PNN_1stRound_08142022_MasterExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/9f/82m1lr2n1fv1mk91plf2l_dr0000gn/T/ch.sudo.cyberduck/c286c8b5-784a-4122-bc7d-bee4738303bc/dcs04/lieber/marmaypag/spatialDLPFC_SCZ_LIBD4100/raw-data/sample_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghokwon/Desktop/Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57E6306-B570-6F4A-9BDD-FF87937C9E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3986E771-8170-F94A-BEB6-C2E793A40CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="960" windowWidth="41180" windowHeight="23180" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
+    <workbookView xWindow="5020" yWindow="960" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Sample #</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">Est. Read Pairs </t>
+  </si>
+  <si>
+    <t>Sample Sheet</t>
   </si>
   <si>
     <t>Experiment #</t>
@@ -261,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +287,15 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -298,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -411,6 +423,15 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -591,12 +612,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -611,31 +632,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -675,39 +696,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -716,6 +737,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,13 +770,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>557868</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>118612</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -789,13 +813,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>135565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>715040</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>177209</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -860,13 +884,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>21264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>715040</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>59364</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -931,13 +955,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6793</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>721833</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>63501</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1002,13 +1026,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>8564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>715040</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>46665</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1073,13 +1097,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>203199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>545168</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>32196</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1117,13 +1141,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>12699</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>360561</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>59070</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1161,13 +1185,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>59070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>367240</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>118139</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1204,13 +1228,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>73398</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>102633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>489810</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>83681</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1645,10 +1669,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView zoomScale="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,705 +1701,735 @@
     <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:24" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+    </row>
+    <row r="2" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C2" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="G2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X2" s="14" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-      <c r="C2" s="32">
-        <v>2719</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="17">
-        <v>14.31</v>
-      </c>
-      <c r="I2" s="17">
-        <v>14</v>
-      </c>
-      <c r="J2" s="17">
-        <v>2099.77</v>
-      </c>
-      <c r="K2" s="17">
-        <f>J2*40/1000</f>
-        <v>83.990800000000007</v>
-      </c>
-      <c r="L2" s="17">
-        <f>K2*0.25</f>
-        <v>20.997700000000002</v>
-      </c>
-      <c r="M2" s="16">
-        <v>17</v>
-      </c>
-      <c r="N2" s="18">
-        <v>459</v>
-      </c>
-      <c r="O2" s="19">
-        <v>2319.39</v>
-      </c>
-      <c r="P2" s="19">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="19">
-        <f>O2*P2</f>
-        <v>27832.68</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="40">
-        <v>100</v>
-      </c>
-      <c r="W2" s="16">
-        <f>((V2/100)*5000*50000)</f>
-        <v>250000000</v>
-      </c>
-      <c r="X2" s="20">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="33">
-        <v>3942</v>
-      </c>
-      <c r="D3" s="38" t="s">
+      <c r="A3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2719</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="4">
-        <v>13.8</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="E3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="17">
+        <v>14.31</v>
+      </c>
+      <c r="I3" s="17">
         <v>14</v>
       </c>
-      <c r="J3" s="4">
-        <v>3321.34</v>
-      </c>
-      <c r="K3" s="4">
-        <f t="shared" ref="K3:K5" si="0">J3*40/1000</f>
-        <v>132.8536</v>
-      </c>
-      <c r="L3" s="4">
-        <f t="shared" ref="L3:L5" si="1">K3*0.25</f>
-        <v>33.2134</v>
-      </c>
-      <c r="M3" s="3">
+      <c r="J3" s="17">
+        <v>2099.77</v>
+      </c>
+      <c r="K3" s="17">
+        <f>J3*40/1000</f>
+        <v>83.990800000000007</v>
+      </c>
+      <c r="L3" s="17">
+        <f>K3*0.25</f>
+        <v>20.997700000000002</v>
+      </c>
+      <c r="M3" s="16">
         <v>17</v>
       </c>
-      <c r="N3" s="3">
-        <v>443</v>
-      </c>
-      <c r="O3" s="5">
-        <v>3413.54</v>
-      </c>
-      <c r="P3" s="5">
+      <c r="N3" s="18">
+        <v>459</v>
+      </c>
+      <c r="O3" s="19">
+        <v>2319.39</v>
+      </c>
+      <c r="P3" s="19">
         <v>12</v>
       </c>
-      <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q5" si="2">O3*P3</f>
-        <v>40962.479999999996</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="Q3" s="19">
+        <f>O3*P3</f>
+        <v>27832.68</v>
+      </c>
+      <c r="R3" s="16" t="s">
         <v>40</v>
       </c>
       <c r="S3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="41">
-        <v>90</v>
-      </c>
-      <c r="W3" s="3">
-        <f>(V3/100)*5000*50000</f>
-        <v>225000000</v>
-      </c>
-      <c r="X3" s="6">
+      <c r="V3" s="40">
+        <v>100</v>
+      </c>
+      <c r="W3" s="16">
+        <f>((V3/100)*5000*50000)</f>
+        <v>250000000</v>
+      </c>
+      <c r="X3" s="20">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="33">
-        <v>5182</v>
+        <v>3942</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4">
-        <v>14.2</v>
+        <v>13.8</v>
       </c>
       <c r="I4" s="4">
         <v>14</v>
       </c>
       <c r="J4" s="4">
+        <v>3321.34</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K6" si="0">J4*40/1000</f>
+        <v>132.8536</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L6" si="1">K4*0.25</f>
+        <v>33.2134</v>
+      </c>
+      <c r="M4" s="3">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3">
+        <v>443</v>
+      </c>
+      <c r="O4" s="5">
+        <v>3413.54</v>
+      </c>
+      <c r="P4" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" ref="Q4:Q6" si="2">O4*P4</f>
+        <v>40962.479999999996</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="41">
+        <v>90</v>
+      </c>
+      <c r="W4" s="3">
+        <f>(V4/100)*5000*50000</f>
+        <v>225000000</v>
+      </c>
+      <c r="X4" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="33">
+        <v>5182</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>14</v>
+      </c>
+      <c r="J5" s="4">
         <v>3090.33</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K5" s="4">
         <f t="shared" si="0"/>
         <v>123.61319999999999</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L5" s="4">
         <f t="shared" si="1"/>
         <v>30.903299999999998</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M5" s="3">
         <v>17</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N5" s="3">
         <v>452</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O5" s="5">
         <v>2885.03</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P5" s="5">
         <v>12</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q5" s="5">
         <f t="shared" si="2"/>
         <v>34620.36</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" s="22" t="s">
+      <c r="R5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="22" t="s">
+      <c r="T5" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="V4" s="41">
+      <c r="U5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="V5" s="41">
         <v>80</v>
       </c>
-      <c r="W4" s="3">
-        <f t="shared" ref="W4:W5" si="3">(V4/100)*5000*50000</f>
+      <c r="W5" s="3">
+        <f t="shared" ref="W5:W6" si="3">(V5/100)*5000*50000</f>
         <v>200000000</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X5" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="7">
+    <row r="6" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C6" s="34">
         <v>5367</v>
       </c>
-      <c r="D5" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D6" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="E6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9">
         <v>13.63</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I6" s="9">
         <v>14</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J6" s="9">
         <v>2861.49</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K6" s="9">
         <f t="shared" si="0"/>
         <v>114.45959999999999</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L6" s="9">
         <f t="shared" si="1"/>
         <v>28.614899999999999</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M6" s="8">
         <v>17</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N6" s="8">
         <v>453</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O6" s="10">
         <v>3684.3</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P6" s="10">
         <v>12</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q6" s="10">
         <f t="shared" si="2"/>
         <v>44211.600000000006</v>
       </c>
-      <c r="R5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="T5" s="23" t="s">
+      <c r="R6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="23" t="s">
+      <c r="T6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="V5" s="42">
+      <c r="U6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" s="42">
         <v>80</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W6" s="8">
         <f t="shared" si="3"/>
         <v>200000000</v>
       </c>
-      <c r="X5" s="11">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="15">
-        <v>5</v>
-      </c>
-      <c r="C6" s="32">
-        <v>1526</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="17">
-        <v>14.16</v>
-      </c>
-      <c r="I6" s="17">
-        <v>14</v>
-      </c>
-      <c r="J6" s="17">
-        <v>1140.95</v>
-      </c>
-      <c r="K6" s="17">
-        <f>J6*40/1000</f>
-        <v>45.637999999999998</v>
-      </c>
-      <c r="L6" s="17">
-        <f>K6*0.25</f>
-        <v>11.4095</v>
-      </c>
-      <c r="M6" s="16">
-        <v>18</v>
-      </c>
-      <c r="N6" s="18">
-        <v>455</v>
-      </c>
-      <c r="O6" s="19">
-        <v>2542.1799999999998</v>
-      </c>
-      <c r="P6" s="19">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="19">
-        <f>O6*P6</f>
-        <v>30506.159999999996</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="V6" s="40">
-        <v>80</v>
-      </c>
-      <c r="W6" s="16">
-        <f>((V6/100)*5000*50000)</f>
-        <v>200000000</v>
-      </c>
-      <c r="X6" s="20">
+      <c r="X6" s="11">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="33">
-        <v>1958</v>
-      </c>
-      <c r="D7" s="38" t="s">
+      <c r="A7" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="C7" s="32">
+        <v>1526</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="17">
+        <v>14.16</v>
+      </c>
+      <c r="I7" s="17">
+        <v>14</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1140.95</v>
+      </c>
+      <c r="K7" s="17">
+        <f>J7*40/1000</f>
+        <v>45.637999999999998</v>
+      </c>
+      <c r="L7" s="17">
+        <f>K7*0.25</f>
+        <v>11.4095</v>
+      </c>
+      <c r="M7" s="16">
         <v>18</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="4">
-        <v>14.1</v>
-      </c>
-      <c r="I7" s="4">
-        <v>14</v>
-      </c>
-      <c r="J7" s="4">
-        <v>2638.2</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" ref="K7:K9" si="4">J7*40/1000</f>
-        <v>105.52800000000001</v>
-      </c>
-      <c r="L7" s="4">
-        <f t="shared" ref="L7:L9" si="5">K7*0.25</f>
-        <v>26.382000000000001</v>
-      </c>
-      <c r="M7" s="3">
-        <v>17</v>
-      </c>
-      <c r="N7" s="3">
-        <v>453</v>
-      </c>
-      <c r="O7" s="5">
-        <v>2867.7</v>
-      </c>
-      <c r="P7" s="5">
+      <c r="N7" s="18">
+        <v>455</v>
+      </c>
+      <c r="O7" s="19">
+        <v>2542.1799999999998</v>
+      </c>
+      <c r="P7" s="19">
         <v>12</v>
       </c>
-      <c r="Q7" s="5">
-        <f t="shared" ref="Q7:Q9" si="6">O7*P7</f>
-        <v>34412.399999999994</v>
-      </c>
-      <c r="R7" s="3" t="s">
+      <c r="Q7" s="19">
+        <f>O7*P7</f>
+        <v>30506.159999999996</v>
+      </c>
+      <c r="R7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="S7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U7" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="T7" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="U7" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="V7" s="41">
-        <v>90</v>
-      </c>
-      <c r="W7" s="3">
-        <f>(V7/100)*5000*50000</f>
-        <v>225000000</v>
-      </c>
-      <c r="X7" s="6">
+      <c r="V7" s="40">
+        <v>80</v>
+      </c>
+      <c r="W7" s="16">
+        <f>((V7/100)*5000*50000)</f>
+        <v>200000000</v>
+      </c>
+      <c r="X7" s="20">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="33">
-        <v>2039</v>
+        <v>1958</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="4">
-        <v>14.05</v>
+        <v>14.1</v>
       </c>
       <c r="I8" s="4">
         <v>14</v>
       </c>
       <c r="J8" s="4">
+        <v>2638.2</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" ref="K8:K10" si="4">J8*40/1000</f>
+        <v>105.52800000000001</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" ref="L8:L10" si="5">K8*0.25</f>
+        <v>26.382000000000001</v>
+      </c>
+      <c r="M8" s="3">
+        <v>17</v>
+      </c>
+      <c r="N8" s="3">
+        <v>453</v>
+      </c>
+      <c r="O8" s="5">
+        <v>2867.7</v>
+      </c>
+      <c r="P8" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" ref="Q8:Q10" si="6">O8*P8</f>
+        <v>34412.399999999994</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="T8" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="U8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="V8" s="41">
+        <v>90</v>
+      </c>
+      <c r="W8" s="3">
+        <f>(V8/100)*5000*50000</f>
+        <v>225000000</v>
+      </c>
+      <c r="X8" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="33">
+        <v>2039</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="I9" s="4">
+        <v>14</v>
+      </c>
+      <c r="J9" s="4">
         <v>1483.41</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K9" s="4">
         <f t="shared" si="4"/>
         <v>59.336400000000005</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L9" s="4">
         <f t="shared" si="5"/>
         <v>14.834100000000001</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M9" s="3">
         <v>18</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N9" s="3">
         <v>443</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O9" s="5">
         <v>3301.55</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P9" s="5">
         <v>12</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q9" s="5">
         <f t="shared" si="6"/>
         <v>39618.600000000006</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="T8" s="22" t="s">
+      <c r="R9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="U8" s="22" t="s">
+      <c r="T9" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="V8" s="41">
+      <c r="U9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="V9" s="41">
         <v>90</v>
       </c>
-      <c r="W8" s="3">
-        <f t="shared" ref="W8:W9" si="7">(V8/100)*5000*50000</f>
+      <c r="W9" s="3">
+        <f t="shared" ref="W9:W10" si="7">(V9/100)*5000*50000</f>
         <v>225000000</v>
       </c>
-      <c r="X8" s="6">
+      <c r="X9" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7">
+    <row r="10" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C10" s="34">
         <v>2378</v>
       </c>
-      <c r="D9" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="D10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="9">
         <v>14.16</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I10" s="9">
         <v>14</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J10" s="9">
         <v>3977.85</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K10" s="9">
         <f t="shared" si="4"/>
         <v>159.114</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L10" s="9">
         <f t="shared" si="5"/>
         <v>39.778500000000001</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M10" s="8">
         <v>17</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N10" s="8">
         <v>455</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O10" s="10">
         <v>3246.73</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P10" s="10">
         <v>12</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q10" s="10">
         <f t="shared" si="6"/>
         <v>38960.76</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="T9" s="23" t="s">
+      <c r="R10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="U9" s="23" t="s">
+      <c r="T10" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="V9" s="42">
+      <c r="U10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="V10" s="42">
         <v>95</v>
       </c>
-      <c r="W9" s="8">
+      <c r="W10" s="8">
         <f t="shared" si="7"/>
         <v>237500000</v>
       </c>
-      <c r="X9" s="11">
+      <c r="X10" s="11">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:X1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -2393,38 +2447,38 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="11:17" x14ac:dyDescent="0.2">
-      <c r="K3" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="43" t="s">
+      <c r="K3" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="44" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="11:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="43"/>
+        <v>31</v>
+      </c>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="44"/>
     </row>
     <row r="5" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K5" s="28">
@@ -2434,7 +2488,7 @@
         <v>2719</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N5" s="4">
         <v>2099.77</v>
@@ -2459,7 +2513,7 @@
         <v>3942</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N6" s="4">
         <v>3321.34</v>
@@ -2484,7 +2538,7 @@
         <v>5182</v>
       </c>
       <c r="M7" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N7" s="4">
         <v>3090.33</v>
@@ -2509,7 +2563,7 @@
         <v>5367</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N8" s="4">
         <v>2861.49</v>
@@ -2534,7 +2588,7 @@
         <v>1526</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N9" s="4">
         <v>1140.95</v>
@@ -2559,7 +2613,7 @@
         <v>1958</v>
       </c>
       <c r="M10" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N10" s="4">
         <v>2638.2</v>
@@ -2584,7 +2638,7 @@
         <v>2039</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N11" s="4">
         <v>1483.41</v>
@@ -2609,7 +2663,7 @@
         <v>2378</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N12" s="4">
         <v>3977.85</v>
@@ -2635,7 +2689,7 @@
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="L3:L4"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2645,7 +2699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216A9C34-C744-764E-B368-A17F0B4ADECD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>

</xml_diff>